<commit_message>
Fixed the code to retreive the config info from AH Fixed the uploading of info to AH, RUN ID 1648
</commit_message>
<xml_diff>
--- a/Data/Temp/Yearly-Report-2021-RO254678.xlsx
+++ b/Data/Temp/Yearly-Report-2021-RO254678.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <x:si>
     <x:t>719333</x:t>
   </x:si>
@@ -176,6 +176,24 @@
   </x:si>
   <x:si>
     <x:t>2017-11-09</x:t>
+  </x:si>
+  <x:si>
+    <x:t>830422</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Professional Services</x:t>
+  </x:si>
+  <x:si>
+    <x:t>252934</x:t>
+  </x:si>
+  <x:si>
+    <x:t>50586.8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>303521</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-12-19</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -787,25 +805,25 @@
     </x:row>
     <x:row r="12" spans="1:7">
       <x:c r="A12" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>1</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="F12" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>